<commit_message>
fix: add step to wait for because timing issue
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/Data_CRM_Verification.xlsx
+++ b/Data Files/Website/DataFiles_CRM/Data_CRM_Verification.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>SearchKYC</t>
   </si>
   <si>
+    <t>requestIdName</t>
+  </si>
+  <si>
     <t>Start_Filterdate</t>
   </si>
   <si>
@@ -91,16 +94,16 @@
     <t>namebefore</t>
   </si>
   <si>
-    <t>10003149</t>
-  </si>
-  <si>
-    <t>20/01/2021</t>
-  </si>
-  <si>
-    <t>02/02/2021</t>
-  </si>
-  <si>
-    <t>Semua</t>
+    <t>RAISA</t>
+  </si>
+  <si>
+    <t>04/05/2021</t>
+  </si>
+  <si>
+    <t>30/06/2021</t>
+  </si>
+  <si>
+    <t>Terverifikasi</t>
   </si>
   <si>
     <t>Test Regression</t>
@@ -109,19 +112,19 @@
     <t>PANCORAN</t>
   </si>
   <si>
-    <t>3171013108850006</t>
-  </si>
-  <si>
-    <t>Deyna Ferrera Corputty</t>
+    <t>3171015504961001</t>
+  </si>
+  <si>
+    <t>TESTING STAGING</t>
   </si>
   <si>
     <t>SURABAYA</t>
   </si>
   <si>
-    <t>31/08/1985</t>
-  </si>
-  <si>
-    <t>LAKI-LAKI</t>
+    <t>15/04/1996</t>
+  </si>
+  <si>
+    <t>PEREMPUAN</t>
   </si>
   <si>
     <t>B</t>
@@ -148,10 +151,10 @@
     <t>WNI</t>
   </si>
   <si>
-    <t>ara</t>
-  </si>
-  <si>
-    <t>31 August 1985</t>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>15 April 1996</t>
   </si>
   <si>
     <t>5/03/2031</t>
@@ -160,7 +163,13 @@
     <t>Without KYC Video</t>
   </si>
   <si>
-    <t>M Habil Ikhwan</t>
+    <t>NURHASANAH</t>
+  </si>
+  <si>
+    <t>3171014605720001</t>
+  </si>
+  <si>
+    <t>Apriani</t>
   </si>
 </sst>
 </file>
@@ -168,10 +177,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -194,9 +203,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,62 +251,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -271,21 +265,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -294,6 +273,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -302,6 +295,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -318,14 +326,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,13 +356,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,13 +464,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,151 +494,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,32 +547,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -578,24 +561,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -624,6 +589,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -638,10 +612,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -650,151 +665,145 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1115,41 +1124,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.0925925925926" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.0925925925926" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.9074074074074" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.8148148148148" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7314814814815" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.2685185185185" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5462962962963" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.9074074074074" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6388888888889" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.1851851851852" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.0925925925926" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9" style="1"/>
-    <col min="17" max="17" width="12.6388888888889" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.9074074074074" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7314814814815" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5462962962963" style="1" customWidth="1"/>
-    <col min="21" max="21" width="16.4537037037037" style="1" customWidth="1"/>
-    <col min="22" max="22" width="21.1851851851852" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15.4259259259259" style="1" customWidth="1"/>
-    <col min="24" max="24" width="18.0925925925926" style="1" customWidth="1"/>
-    <col min="25" max="25" width="27.9074074074074" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="9" style="1"/>
+    <col min="1" max="3" width="19" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.0925925925926" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.0925925925926" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.9074074074074" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.8148148148148" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7314814814815" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.2685185185185" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5462962962963" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.9074074074074" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6388888888889" style="1" customWidth="1"/>
+    <col min="14" max="14" width="26.1851851851852" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.0925925925926" style="1" customWidth="1"/>
+    <col min="16" max="17" width="9" style="1"/>
+    <col min="18" max="18" width="12.6388888888889" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.9074074074074" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7314814814815" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5462962962963" style="1" customWidth="1"/>
+    <col min="22" max="22" width="16.4537037037037" style="1" customWidth="1"/>
+    <col min="23" max="23" width="21.1851851851852" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15.4259259259259" style="1" customWidth="1"/>
+    <col min="25" max="25" width="18.0925925925926" style="1" customWidth="1"/>
+    <col min="26" max="26" width="27.9074074074074" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1225,18 +1234,21 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" ht="28.8" spans="1:25">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" ht="28.8" spans="1:26">
+      <c r="A2" s="2">
+        <v>10003387</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1263,14 +1275,14 @@
       <c r="L2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>39</v>
@@ -1293,14 +1305,97 @@
       <c r="V2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="6" t="s">
         <v>47</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" ht="28.8" spans="1:26">
+      <c r="A3" s="2">
+        <v>10003387</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update flaky test step
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/Data_CRM_Verification.xlsx
+++ b/Data Files/Website/DataFiles_CRM/Data_CRM_Verification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9480"/>
+    <workbookView windowWidth="9432" windowHeight="8735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>SearchKYC</t>
   </si>
@@ -94,13 +94,13 @@
     <t>namebefore</t>
   </si>
   <si>
-    <t>RAISA</t>
-  </si>
-  <si>
-    <t>04/05/2021</t>
-  </si>
-  <si>
-    <t>30/06/2021</t>
+    <t>TESTING STAGING</t>
+  </si>
+  <si>
+    <t>04/02/2021</t>
+  </si>
+  <si>
+    <t>30/05/2021</t>
   </si>
   <si>
     <t>Terverifikasi</t>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>3171015504961001</t>
-  </si>
-  <si>
-    <t>TESTING STAGING</t>
   </si>
   <si>
     <t>SURABAYA</t>
@@ -177,10 +174,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -203,6 +200,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -211,49 +237,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -265,6 +269,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -273,15 +284,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,12 +302,34 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -311,37 +338,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,13 +353,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,19 +503,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,145 +527,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,6 +544,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -592,47 +619,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,10 +635,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -662,136 +662,133 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1127,7 +1124,7 @@
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1240,7 +1237,7 @@
     </row>
     <row r="2" ht="28.8" spans="1:26">
       <c r="A2" s="2">
-        <v>10003387</v>
+        <v>10003572</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>26</v>
@@ -1264,63 +1261,63 @@
         <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" ht="28.8" spans="1:26">
       <c r="A3" s="2">
-        <v>10003387</v>
+        <v>10003572</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
@@ -1341,61 +1338,61 @@
         <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>